<commit_message>
learn about array in java
</commit_message>
<xml_diff>
--- a/Class-Updates-Tracker-Java.xlsx
+++ b/Class-Updates-Tracker-Java.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\java utube\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15FB7B4A-E62C-45D9-AEF6-6C61537FCC90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{392237B8-EA31-408D-AA49-1B9C7A9797DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
   <si>
     <t>video</t>
   </si>
@@ -103,6 +103,22 @@
   </si>
   <si>
     <t>https://youtu.be/0r1SfRoLuzU</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>https://youtu.be/ITr0uX2Ez1o</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>array and how to make array and how to insert array and solve some question</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>https://youtu.be/qqRDHzPli3o</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>https://youtu.be/aSGa3S2-sQ0</t>
     <phoneticPr fontId="5"/>
   </si>
 </sst>
@@ -180,7 +196,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -240,12 +256,62 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -269,6 +335,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -577,10 +655,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="B1:E62"/>
+  <dimension ref="B1:I62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -590,11 +668,12 @@
     <col min="3" max="3" width="117" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="62.54296875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="50.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="2" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="3" spans="2:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="1" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="2:9" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.7">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -608,7 +687,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:5" ht="39.75" customHeight="1" x14ac:dyDescent="1">
+    <row r="4" spans="2:9" ht="39.75" customHeight="1" x14ac:dyDescent="1">
       <c r="C4" s="3" t="s">
         <v>4</v>
       </c>
@@ -619,7 +698,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="2:5" ht="24" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="2:9" ht="24" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B5" s="4" t="s">
         <v>5</v>
       </c>
@@ -633,7 +712,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="2:5" ht="24" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="2:9" ht="24" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B6" s="4" t="s">
         <v>9</v>
       </c>
@@ -647,7 +726,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="2:5" ht="24" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="2:9" ht="24" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B7" s="4" t="s">
         <v>13</v>
       </c>
@@ -659,7 +738,7 @@
       </c>
       <c r="E7" s="5"/>
     </row>
-    <row r="8" spans="2:5" ht="24" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="2:9" ht="24" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B8" s="4" t="s">
         <v>16</v>
       </c>
@@ -673,7 +752,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="2:5" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:9" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="4" t="s">
         <v>20</v>
       </c>
@@ -687,15 +766,27 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="2:5" ht="24" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="2:9" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="5"/>
-    </row>
-    <row r="11" spans="2:5" ht="24" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="C10" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="11"/>
+    </row>
+    <row r="11" spans="2:9" ht="24" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B11" s="4" t="s">
         <v>22</v>
       </c>
@@ -703,7 +794,7 @@
       <c r="D11" s="6"/>
       <c r="E11" s="5"/>
     </row>
-    <row r="12" spans="2:5" ht="24" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="2:9" ht="24" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B12" s="4" t="s">
         <v>23</v>
       </c>
@@ -711,25 +802,25 @@
       <c r="D12" s="6"/>
       <c r="E12" s="5"/>
     </row>
-    <row r="13" spans="2:5" ht="24" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="2:9" ht="24" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B13" s="4"/>
       <c r="C13" s="5"/>
       <c r="D13" s="6"/>
       <c r="E13" s="5"/>
     </row>
-    <row r="14" spans="2:5" ht="24" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="2:9" ht="24" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B14" s="4"/>
       <c r="C14" s="5"/>
       <c r="D14" s="6"/>
       <c r="E14" s="5"/>
     </row>
-    <row r="15" spans="2:5" ht="24" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="2:9" ht="24" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B15" s="4"/>
       <c r="C15" s="5"/>
       <c r="D15" s="6"/>
       <c r="E15" s="5"/>
     </row>
-    <row r="16" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="18" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="19" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -779,10 +870,16 @@
     <row r="61" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="62" spans="2:2" ht="28.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="F10:I10"/>
+  </mergeCells>
   <phoneticPr fontId="5"/>
   <hyperlinks>
     <hyperlink ref="D9" r:id="rId1" xr:uid="{DF269509-726B-4C5C-9333-9446C5C21ECE}"/>
-    <hyperlink ref="E9" r:id="rId2" xr:uid="{8E9EC36F-3F87-451C-A752-2521C593A2BC}"/>
+    <hyperlink ref="D10" r:id="rId2" xr:uid="{FF7E07CF-23E0-47CD-B6D1-B1A4E392A378}"/>
+    <hyperlink ref="E9" r:id="rId3" xr:uid="{8E9EC36F-3F87-451C-A752-2521C593A2BC}"/>
+    <hyperlink ref="E10" r:id="rId4" xr:uid="{4662B24C-6362-4A05-B0C4-E96F39915972}"/>
+    <hyperlink ref="F10" r:id="rId5" xr:uid="{C878FBEC-BEBE-4CD4-B890-B1BC9E75BFF0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
learan about method and what is mean by public  static void main
</commit_message>
<xml_diff>
--- a/Class-Updates-Tracker-Java.xlsx
+++ b/Class-Updates-Tracker-Java.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\java utube\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{392237B8-EA31-408D-AA49-1B9C7A9797DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF2889FE-0B08-4F3B-B790-4CEBB4516B38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
   <si>
     <t>video</t>
   </si>
@@ -119,6 +119,10 @@
   </si>
   <si>
     <t>https://youtu.be/aSGa3S2-sQ0</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>extra supported video2</t>
     <phoneticPr fontId="5"/>
   </si>
 </sst>
@@ -271,30 +275,34 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </left>
-      <right/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
+      <left style="thin">
         <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
+      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -340,13 +348,13 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -655,10 +663,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="B1:I62"/>
+  <dimension ref="B1:F62"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -668,12 +676,12 @@
     <col min="3" max="3" width="117" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="62.54296875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="50.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.7265625" customWidth="1"/>
+    <col min="6" max="6" width="41.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="2" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="3" spans="2:9" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.7">
+    <row r="1" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="2:6" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.7">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -686,8 +694,11 @@
       <c r="E3" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="2:9" ht="39.75" customHeight="1" x14ac:dyDescent="1">
+      <c r="F3" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" ht="39.75" customHeight="1" x14ac:dyDescent="1">
       <c r="C4" s="3" t="s">
         <v>4</v>
       </c>
@@ -697,8 +708,11 @@
       <c r="E4" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="2:9" ht="24" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="F4" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B5" s="4" t="s">
         <v>5</v>
       </c>
@@ -711,8 +725,9 @@
       <c r="E5" s="6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="2:9" ht="24" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="F5" s="6"/>
+    </row>
+    <row r="6" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B6" s="4" t="s">
         <v>9</v>
       </c>
@@ -725,8 +740,9 @@
       <c r="E6" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="7" spans="2:9" ht="24" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="F6" s="6"/>
+    </row>
+    <row r="7" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B7" s="4" t="s">
         <v>13</v>
       </c>
@@ -737,8 +753,9 @@
         <v>15</v>
       </c>
       <c r="E7" s="5"/>
-    </row>
-    <row r="8" spans="2:9" ht="24" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="F7" s="5"/>
+    </row>
+    <row r="8" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B8" s="4" t="s">
         <v>16</v>
       </c>
@@ -751,8 +768,9 @@
       <c r="E8" s="6" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="9" spans="2:9" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F8" s="6"/>
+    </row>
+    <row r="9" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="4" t="s">
         <v>20</v>
       </c>
@@ -762,65 +780,68 @@
       <c r="D9" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="E9" s="10" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="10" spans="2:9" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F9" s="10"/>
+    </row>
+    <row r="10" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="4" t="s">
         <v>21</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="E10" s="9" t="s">
+      <c r="E10" s="12" t="s">
         <v>29</v>
       </c>
       <c r="F10" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="11"/>
-    </row>
-    <row r="11" spans="2:9" ht="24" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="11" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B11" s="4" t="s">
         <v>22</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="6"/>
-      <c r="E11" s="5"/>
-    </row>
-    <row r="12" spans="2:9" ht="24" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+    </row>
+    <row r="12" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B12" s="4" t="s">
         <v>23</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="6"/>
-      <c r="E12" s="5"/>
-    </row>
-    <row r="13" spans="2:9" ht="24" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+    </row>
+    <row r="13" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B13" s="4"/>
       <c r="C13" s="5"/>
       <c r="D13" s="6"/>
       <c r="E13" s="5"/>
-    </row>
-    <row r="14" spans="2:9" ht="24" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="F13" s="5"/>
+    </row>
+    <row r="14" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B14" s="4"/>
       <c r="C14" s="5"/>
       <c r="D14" s="6"/>
       <c r="E14" s="5"/>
-    </row>
-    <row r="15" spans="2:9" ht="24" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="F14" s="5"/>
+    </row>
+    <row r="15" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B15" s="4"/>
       <c r="C15" s="5"/>
       <c r="D15" s="6"/>
       <c r="E15" s="5"/>
-    </row>
-    <row r="16" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="F15" s="5"/>
+    </row>
+    <row r="16" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="18" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="19" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -870,16 +891,13 @@
     <row r="61" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="62" spans="2:2" ht="28.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="F10:I10"/>
-  </mergeCells>
   <phoneticPr fontId="5"/>
   <hyperlinks>
     <hyperlink ref="D9" r:id="rId1" xr:uid="{DF269509-726B-4C5C-9333-9446C5C21ECE}"/>
     <hyperlink ref="D10" r:id="rId2" xr:uid="{FF7E07CF-23E0-47CD-B6D1-B1A4E392A378}"/>
     <hyperlink ref="E9" r:id="rId3" xr:uid="{8E9EC36F-3F87-451C-A752-2521C593A2BC}"/>
     <hyperlink ref="E10" r:id="rId4" xr:uid="{4662B24C-6362-4A05-B0C4-E96F39915972}"/>
-    <hyperlink ref="F10" r:id="rId5" xr:uid="{C878FBEC-BEBE-4CD4-B890-B1BC9E75BFF0}"/>
+    <hyperlink ref="F10" r:id="rId5" xr:uid="{8A344E58-E167-420E-9C96-8E11789B88BD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
learn about static keyword
</commit_message>
<xml_diff>
--- a/Class-Updates-Tracker-Java.xlsx
+++ b/Class-Updates-Tracker-Java.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\java utube\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF2889FE-0B08-4F3B-B790-4CEBB4516B38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DB1CA33-2FA1-4150-9EA3-8A1F7DD17E22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="34">
   <si>
     <t>video</t>
   </si>
@@ -123,6 +123,14 @@
   </si>
   <si>
     <t>extra supported video2</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>https://youtu.be/ZnfOBRS7KCg</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>learn about method and what is mean by public static void main in java</t>
     <phoneticPr fontId="5"/>
   </si>
 </sst>
@@ -666,7 +674,7 @@
   <dimension ref="B1:F62"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -802,12 +810,16 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="6"/>
+      <c r="C11" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>32</v>
+      </c>
       <c r="E11" s="11"/>
       <c r="F11" s="11"/>
     </row>
@@ -898,6 +910,7 @@
     <hyperlink ref="E9" r:id="rId3" xr:uid="{8E9EC36F-3F87-451C-A752-2521C593A2BC}"/>
     <hyperlink ref="E10" r:id="rId4" xr:uid="{4662B24C-6362-4A05-B0C4-E96F39915972}"/>
     <hyperlink ref="F10" r:id="rId5" xr:uid="{8A344E58-E167-420E-9C96-8E11789B88BD}"/>
+    <hyperlink ref="D11" r:id="rId6" xr:uid="{45ACF002-962E-41BF-92DC-1CA7653639E8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
learn about class object method overloading and constructor in java
</commit_message>
<xml_diff>
--- a/Class-Updates-Tracker-Java.xlsx
+++ b/Class-Updates-Tracker-Java.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\java utube\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DB1CA33-2FA1-4150-9EA3-8A1F7DD17E22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F33093BE-EA4F-4902-BB3F-8B0DE524DB9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="38">
   <si>
     <t>video</t>
   </si>
@@ -131,6 +131,21 @@
   </si>
   <si>
     <t>learn about method and what is mean by public static void main in java</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>https://youtu.be/K9Rvor70Aiw</t>
+  </si>
+  <si>
+    <t>day9</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>oops start and learn about class and objects ,methodoverloading,consturctor and this keyword in java</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>lean about static keyword in details</t>
     <phoneticPr fontId="5"/>
   </si>
 </sst>
@@ -671,10 +686,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="B1:F62"/>
+  <dimension ref="B1:F71"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -827,14 +842,22 @@
       <c r="B12" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="5"/>
-      <c r="D12" s="6"/>
+      <c r="C12" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
     </row>
     <row r="13" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B13" s="4"/>
-      <c r="C13" s="5"/>
+      <c r="B13" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>36</v>
+      </c>
       <c r="D13" s="6"/>
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
@@ -853,23 +876,77 @@
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
     </row>
-    <row r="16" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="17" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="18" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="19" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="20" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="21" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="22" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="24" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="25" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="27" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="28" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="29" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="30" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="31" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="32" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B16" s="4"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+    </row>
+    <row r="17" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B17" s="4"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+    </row>
+    <row r="18" spans="2:6" ht="23" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B18" s="4"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+    </row>
+    <row r="19" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B19" s="4"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+    </row>
+    <row r="20" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B20" s="4"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+    </row>
+    <row r="21" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B21" s="4"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+    </row>
+    <row r="22" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B22" s="4"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+    </row>
+    <row r="23" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B23" s="4"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+    </row>
+    <row r="24" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B24" s="4"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+    </row>
+    <row r="25" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="33" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="34" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="35" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -883,25 +960,34 @@
     <row r="43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="44" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="45" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="46" ht="31.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="46" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="47" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="48" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="49" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="50" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="51" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="52" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="53" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B53" s="7"/>
-    </row>
+    <row r="53" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="54" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="55" spans="2:2" ht="15.65" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="55" spans="2:2" ht="31.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="56" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="57" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="58" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="59" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="60" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="61" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="62" spans="2:2" ht="28.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="62" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B62" s="7"/>
+    </row>
+    <row r="63" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="64" spans="2:2" ht="15.65" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="65" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="66" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="67" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="68" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="69" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="70" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="71" ht="28.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <phoneticPr fontId="5"/>
   <hyperlinks>

</xml_diff>

<commit_message>
piller1-learn about inheritance,methodoverriding,super and final key in java
</commit_message>
<xml_diff>
--- a/Class-Updates-Tracker-Java.xlsx
+++ b/Class-Updates-Tracker-Java.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\java utube\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F33093BE-EA4F-4902-BB3F-8B0DE524DB9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D0B2BF8-1E20-4563-A34C-446F173A5706}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="46">
   <si>
     <t>video</t>
   </si>
@@ -79,74 +79,104 @@
     <t>https://youtu.be/PmLaWONTWKc</t>
   </si>
   <si>
+    <t>Day5</t>
+  </si>
+  <si>
+    <t>Day7</t>
+  </si>
+  <si>
+    <t>Day8</t>
+  </si>
+  <si>
+    <t>learn about loop (for loop, while loop and do-while loop)</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>https://youtu.be/30xvczNMAUs</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>https://youtu.be/0r1SfRoLuzU</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>https://youtu.be/ITr0uX2Ez1o</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>array and how to make array and how to insert array and solve some question</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>https://youtu.be/qqRDHzPli3o</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>https://youtu.be/aSGa3S2-sQ0</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>extra supported video2</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>https://youtu.be/ZnfOBRS7KCg</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>learn about method and what is mean by public static void main in java</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>https://youtu.be/K9Rvor70Aiw</t>
+  </si>
+  <si>
+    <t>lean about static keyword in details</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>oops start and learn about class and objects ,methodoverloading andconsturctor  java</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>https://youtu.be/E98I2pky-hQ</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>this keyword in java</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>https://youtu.be/DzHGyfZH6fA</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>Day6</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>Day9</t>
+  </si>
+  <si>
+    <t>Day10</t>
+  </si>
+  <si>
+    <t>Day11</t>
+  </si>
+  <si>
     <t>https://youtu.be/AmiV9r7ILQI</t>
-  </si>
-  <si>
-    <t>Day5</t>
-  </si>
-  <si>
-    <t>Day6</t>
-  </si>
-  <si>
-    <t>Day7</t>
-  </si>
-  <si>
-    <t>Day8</t>
-  </si>
-  <si>
-    <t>learn about loop (for loop, while loop and do-while loop)</t>
-    <phoneticPr fontId="5"/>
-  </si>
-  <si>
-    <t>https://youtu.be/30xvczNMAUs</t>
-    <phoneticPr fontId="5"/>
-  </si>
-  <si>
-    <t>https://youtu.be/0r1SfRoLuzU</t>
-    <phoneticPr fontId="5"/>
-  </si>
-  <si>
-    <t>https://youtu.be/ITr0uX2Ez1o</t>
-    <phoneticPr fontId="5"/>
-  </si>
-  <si>
-    <t>array and how to make array and how to insert array and solve some question</t>
-    <phoneticPr fontId="5"/>
-  </si>
-  <si>
-    <t>https://youtu.be/qqRDHzPli3o</t>
-    <phoneticPr fontId="5"/>
-  </si>
-  <si>
-    <t>https://youtu.be/aSGa3S2-sQ0</t>
-    <phoneticPr fontId="5"/>
-  </si>
-  <si>
-    <t>extra supported video2</t>
-    <phoneticPr fontId="5"/>
-  </si>
-  <si>
-    <t>https://youtu.be/ZnfOBRS7KCg</t>
-    <phoneticPr fontId="5"/>
-  </si>
-  <si>
-    <t>learn about method and what is mean by public static void main in java</t>
-    <phoneticPr fontId="5"/>
-  </si>
-  <si>
-    <t>https://youtu.be/K9Rvor70Aiw</t>
-  </si>
-  <si>
-    <t>day9</t>
-    <phoneticPr fontId="5"/>
-  </si>
-  <si>
-    <t>oops start and learn about class and objects ,methodoverloading,consturctor and this keyword in java</t>
-    <phoneticPr fontId="5"/>
-  </si>
-  <si>
-    <t>lean about static keyword in details</t>
-    <phoneticPr fontId="5"/>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>learn about if-else and switch in java</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>https://youtu.be/OTMsKM8OZNQ</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>Day12</t>
   </si>
 </sst>
 </file>
@@ -342,7 +372,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -378,6 +408,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -686,10 +719,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="B1:F71"/>
+  <dimension ref="B1:F72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -718,7 +751,7 @@
         <v>3</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="2:6" ht="39.75" customHeight="1" x14ac:dyDescent="1">
@@ -788,96 +821,112 @@
       <c r="D8" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="F8" s="6"/>
+    </row>
+    <row r="9" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B9" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F8" s="6"/>
-    </row>
-    <row r="9" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="4" t="s">
-        <v>20</v>
-      </c>
       <c r="C9" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+    </row>
+    <row r="10" spans="2:6" ht="22" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="F9" s="10"/>
-    </row>
-    <row r="10" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="E10" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="F10" s="12" t="s">
-        <v>30</v>
-      </c>
+      <c r="F10" s="10"/>
     </row>
     <row r="11" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-    </row>
-    <row r="12" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+        <v>26</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
+        <v>31</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
     </row>
     <row r="13" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B13" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+    </row>
+    <row r="14" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C13" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="D13" s="6"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-    </row>
-    <row r="14" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B14" s="4"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="6"/>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B15" s="4"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="6"/>
+    <row r="15" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>37</v>
+      </c>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
     </row>
     <row r="16" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B16" s="4"/>
+      <c r="B16" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="C16" s="5"/>
       <c r="D16" s="6"/>
       <c r="E16" s="5"/>
@@ -890,14 +939,14 @@
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
     </row>
-    <row r="18" spans="2:6" ht="23" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B18" s="4"/>
       <c r="C18" s="5"/>
       <c r="D18" s="6"/>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
     </row>
-    <row r="19" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="2:6" ht="23" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B19" s="4"/>
       <c r="C19" s="5"/>
       <c r="D19" s="6"/>
@@ -939,7 +988,13 @@
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
     </row>
-    <row r="25" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B25" s="4"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+    </row>
     <row r="26" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="27" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="28" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -969,34 +1024,39 @@
     <row r="52" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="53" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="54" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="55" spans="2:2" ht="31.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="56" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="55" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="56" spans="2:2" ht="31.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="57" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="58" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="59" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="60" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="61" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="62" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B62" s="7"/>
-    </row>
-    <row r="63" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="64" spans="2:2" ht="15.65" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="65" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="62" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="63" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B63" s="7"/>
+    </row>
+    <row r="64" spans="2:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="65" ht="15.65" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="66" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="67" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="68" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="69" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="70" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="71" ht="28.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="71" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="72" ht="28.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <phoneticPr fontId="5"/>
   <hyperlinks>
-    <hyperlink ref="D9" r:id="rId1" xr:uid="{DF269509-726B-4C5C-9333-9446C5C21ECE}"/>
-    <hyperlink ref="D10" r:id="rId2" xr:uid="{FF7E07CF-23E0-47CD-B6D1-B1A4E392A378}"/>
-    <hyperlink ref="E9" r:id="rId3" xr:uid="{8E9EC36F-3F87-451C-A752-2521C593A2BC}"/>
-    <hyperlink ref="E10" r:id="rId4" xr:uid="{4662B24C-6362-4A05-B0C4-E96F39915972}"/>
-    <hyperlink ref="F10" r:id="rId5" xr:uid="{8A344E58-E167-420E-9C96-8E11789B88BD}"/>
-    <hyperlink ref="D11" r:id="rId6" xr:uid="{45ACF002-962E-41BF-92DC-1CA7653639E8}"/>
+    <hyperlink ref="D10" r:id="rId1" xr:uid="{DF269509-726B-4C5C-9333-9446C5C21ECE}"/>
+    <hyperlink ref="D11" r:id="rId2" xr:uid="{FF7E07CF-23E0-47CD-B6D1-B1A4E392A378}"/>
+    <hyperlink ref="E10" r:id="rId3" xr:uid="{8E9EC36F-3F87-451C-A752-2521C593A2BC}"/>
+    <hyperlink ref="E11" r:id="rId4" xr:uid="{4662B24C-6362-4A05-B0C4-E96F39915972}"/>
+    <hyperlink ref="F11" r:id="rId5" xr:uid="{8A344E58-E167-420E-9C96-8E11789B88BD}"/>
+    <hyperlink ref="D12" r:id="rId6" xr:uid="{45ACF002-962E-41BF-92DC-1CA7653639E8}"/>
+    <hyperlink ref="D14" r:id="rId7" xr:uid="{9FD94FC2-C602-4E71-AD25-2975A6ECDC53}"/>
+    <hyperlink ref="D15" r:id="rId8" xr:uid="{959E257A-0147-4C90-97D9-5042C0D6C251}"/>
+    <hyperlink ref="E8" r:id="rId9" xr:uid="{649FA6F5-AE0A-40F0-B9B0-3F91F8534DAE}"/>
+    <hyperlink ref="D9" r:id="rId10" xr:uid="{F1FD8ACC-B4B3-44C1-B1FA-B2E92E167D3C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
piller2-polymorphism learn about runtime(overriding)compile(method overloading)
</commit_message>
<xml_diff>
--- a/Class-Updates-Tracker-Java.xlsx
+++ b/Class-Updates-Tracker-Java.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\java utube\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D0B2BF8-1E20-4563-A34C-446F173A5706}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA4C20E4-26DC-4645-B5E5-38705AC4F1F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="48">
   <si>
     <t>video</t>
   </si>
@@ -177,6 +177,14 @@
   </si>
   <si>
     <t>Day12</t>
+  </si>
+  <si>
+    <t>oops piller1-learn about inheritance(extend key),method overriding,super key and final key in java</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>https://youtu.be/UrmbrygUyzU</t>
+    <phoneticPr fontId="5"/>
   </si>
 </sst>
 </file>
@@ -721,8 +729,8 @@
   </sheetPr>
   <dimension ref="B1:F72"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -923,12 +931,16 @@
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
     </row>
-    <row r="16" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="2:6" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C16" s="5"/>
-      <c r="D16" s="6"/>
+      <c r="C16" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>47</v>
+      </c>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
     </row>
@@ -1057,6 +1069,7 @@
     <hyperlink ref="D15" r:id="rId8" xr:uid="{959E257A-0147-4C90-97D9-5042C0D6C251}"/>
     <hyperlink ref="E8" r:id="rId9" xr:uid="{649FA6F5-AE0A-40F0-B9B0-3F91F8534DAE}"/>
     <hyperlink ref="D9" r:id="rId10" xr:uid="{F1FD8ACC-B4B3-44C1-B1FA-B2E92E167D3C}"/>
+    <hyperlink ref="D16" r:id="rId11" xr:uid="{47F67C17-75C3-47D0-BCE3-0D20E3D624D0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>